<commit_message>
data double check - part 2
finish data extraction and double check
</commit_message>
<xml_diff>
--- a/doublecheck/Data extraction of PT-JAO-RH edit.xlsx
+++ b/doublecheck/Data extraction of PT-JAO-RH edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tired_llama\projects\bahmani-sysrev\doublecheck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0A6339-949D-40F5-A5AC-99410D955B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F8A9E0-88D3-4EB0-AFF1-505EBD48125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,17 +445,6 @@
     <t>43 Total knee arthroplasty or 40 Total hip arthroplasty</t>
   </si>
   <si>
-    <t>Temperament and Character Inventory</t>
-  </si>
-  <si>
-    <t>higher pre-operative
-harm avoidance, persistence, and anxiety scores were
-predictive of residual pain after THA and TKA (-2log
-Likelihood = 63.267; R2
-Nagelkerke = 0.349; X2 = 20.897;
-df = 3; p &lt; 0.001).</t>
-  </si>
-  <si>
     <t xml:space="preserve"> SF-12, HADS, VAS, HHS, KSS, and WOMAC </t>
   </si>
   <si>
@@ -472,9 +461,6 @@
   </si>
   <si>
     <t>Minimum follow-up period was two years</t>
-  </si>
-  <si>
-    <t>Satisfied patients showed significantly higher scores for life satisfaction (𝑝 = 0.006) and performance orientation (𝑝 = 0.015), whereas dissatisfied patients showed significantly higher scores for somatic distress (𝑝 = 0.001) and emotional instability (𝑝 = 0.002). no significant differences were found in the other personality traits of the FPI-R</t>
   </si>
   <si>
     <t>satisfiction</t>
@@ -516,9 +502,6 @@
   </si>
   <si>
     <t>1 week before surgery + 1 and 6 months after surgery</t>
-  </si>
-  <si>
-    <t>The Knee Society Score (KSS), The Short-Form Health Survey questionnaire (SF-36) are affected by negative emotions, including neuroticism, anxiety, and depression</t>
   </si>
   <si>
     <t>KSS, SF-36</t>
@@ -544,9 +527,6 @@
 of each personality type impact recovery</t>
   </si>
   <si>
-    <t>n=387, age=59.6, male=109, BMI=27.8</t>
-  </si>
-  <si>
     <t>Eysenck Personality
 Questionnaire (EPQ)</t>
   </si>
@@ -571,9 +551,6 @@
     <t>average 24.6 months postoperatively</t>
   </si>
   <si>
-    <t>sanguine group had the highest QALYs and change of total WOMAC scores but had the lowest postoperative WOMAC and MCER in comparison with other traits (all P &lt; 0.05) Melancholic group had the lowest QALYs and changeof total WOMAC scores but had the highest postoperative WOMAC and MCER in comparison with other traits(all P &lt; 0.05).</t>
-  </si>
-  <si>
     <t>WOMAC</t>
   </si>
   <si>
@@ -595,39 +572,10 @@
     <t>52, 67.19+-7.68, male= 26.9%, not mentioned</t>
   </si>
   <si>
-    <t>n=488,revision=196,n=67.4,revN=67.8,male=42.6%,malerevN=46.9%,bmi25%&lt;&lt;25</t>
-  </si>
-  <si>
     <t>total hip arthroplastyl and revision THA</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Optimism-Pessimism (PSM) scale of the Minnesota</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Multiphasic Personality Inventory
-(MMPI) questionnaire </t>
-    </r>
-  </si>
-  <si>
     <t>2 years postoperative</t>
-  </si>
-  <si>
-    <t>single-item pain assessment(self-reported hip pain and hip function compared to condition before surgery) was used in order to measure outcome</t>
-  </si>
-  <si>
-    <t>12.3 % of pessimists versus 8 % of non-pessimists had moderate-severe pain 2-years after primary THA leading to an odds ratio of 2.16 (95 % CI: 0.90, 5.20; p = 0.08).Improvement in Hip Function to “Better/Same/Worse” vs. “Much Better” OR=1.87 (95%cl=0.77, 4.52) P= 0.16. Moderate-Severe Activity Limitation vs. None-Mild Activity Limitation OR= 2.90 (95 % CI: 1.25, 6.70) p= 0.01.in pessimists compared to non-pessimists in the multivariable adjusted logistic model Pessimists were not significantly different than nonpessimists to report moderate-severe pain, lack of “much better” improvement in hip function or moderate-severe activity limitation 2 years post-revision THA, ORs were1.18 (95 % CI: 0.50, 2.81; p = 0.71), 1.08 (95 % CI: 0.52,2.27; p = 0.83) and 1.73 (95 % CI: 0.76, 3.94; p = 0.19), respectively.</t>
   </si>
   <si>
     <t>retrospective cohort study</t>
@@ -637,76 +585,19 @@
 patients with different personality traits.</t>
   </si>
   <si>
-    <r>
-      <t>n=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>232</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>. age=between 46 and 71,male=105,bmi=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>27.1</t>
-    </r>
-  </si>
-  <si>
-    <t>costeffectiveness ratio (MCER), quality-adjusted life years (QALYs), McMaster Universities Osteoarthritis Index were measured (WOMAC) questionnaire, EPQ</t>
-  </si>
-  <si>
     <t>1 week before to 6 months after surgery</t>
   </si>
   <si>
-    <t xml:space="preserve">SF-36 PCS  and Extraversion 0.62 correlation p=0.040
-SF-36 MCS  and neuroticism -0.62 correlation p=0.018
-WOMAC pain Extraversion -0.64 correlation p=0.018
-WOMAC pain neuroticism -0.71 correlation p=0.025.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> to determine whether psychological factors affect health-related quality of life (HRQL) and recovery of knee
-function in total knee replacement (TKR) patients</t>
-  </si>
-  <si>
     <t>prospective clinical controlled study</t>
   </si>
   <si>
-    <t xml:space="preserve">n=80 ,mean age=66 , gender= 32 male 60%female ,BMI=satisfied28.6  dissatisfied28 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VAS, WOMAC, Knee clinical score KSS, Function score KSS, ROM and Stability was used in order to measure satisfaction and dissatisfaction following operation
-</t>
-  </si>
-  <si>
     <t>To evaluate if presence of some psychiatric disorders or personality traits could be the main cause for the worse outcome of total knee arthroplasty in patients with allergies</t>
   </si>
   <si>
-    <t>n=209 , age=72.84 (SD 8.32), male=68, 33%, BMI= 31.37 (SD 4.67)</t>
-  </si>
-  <si>
     <t>reduced NEO Inventory of Five-Factor  (NEO-FFI)</t>
   </si>
   <si>
     <t>preoperative and 6 months after the operation</t>
-  </si>
-  <si>
-    <t>83total, 40tha, 43tka, 67.67 +-10.6,65.6+-10.6tha,69.6+-7.8tka,male=44.57%,22.55%tha,15.35%tka, in TKA,32.3 +-5.7, in THA 27.8 +- 4.8</t>
   </si>
   <si>
     <t>,preoperative,5 days, and 1, 3, 6 and 12 month</t>
@@ -720,20 +611,6 @@
   </si>
   <si>
     <t>2weeks before and 6 months after surgery</t>
-  </si>
-  <si>
-    <t>residual pain (30&lt;VAS) was noted in 15% of the THA patients and 25% of the TKA patients, and it
-correlated with, functionality and WOMAC ,SF-12 and HADS scores at t5 .  high levels of preoperative harm avoidance and persistence were predictive
-of residual Postoperative pain</t>
-  </si>
-  <si>
-    <t>sf-12 score, womac, KSS  were measured. At 6 months of follow up, patients with referred allergies presented worse outcomes for most of the scores (SF-12physical, WOMAC-total score and WOMAC-pain, and function sub-scores)      anxiety is more prevalent in the group of patients with reported allergies</t>
-  </si>
-  <si>
-    <t>anxiety is more prevalent in the group
-of patients with reported allergies(STAI-T,  p = 0.039) 
-WOMAC (total) had correlation with postoperatiove allergy(p=0.046) 
-WOMAC-pain had correlation with posoperative allergy(p=0.013)  SF-12 physical had corelation with posoperative allergy(p=0.004). womac function p=0.012 had correlated with allergy</t>
   </si>
   <si>
     <t>knee function 6 months after surgery(KSS) was negatively associated with trait anxiety inventory and neuroticism(both P&lt;0.05), but positively associated with extraversion(P&lt;0.05).     Preoperative PhysicalComponent Summary Scale (PCS) and Mental Component Summary Scale (MCS) scores were negatively associated with extraversion (E score) (B=–0.986 and –0.967, respectively, both P&lt;0.05).   Postoperative PCS and State Anxiety Inventory (SAI)
@@ -956,12 +833,190 @@
 The mean EQ-5D score one year post-operative was 0.72 for the THA group and 0.67 for the TKA group.
 There was a significant difference in the EQ-5D score between the two groups one year post-operative (p=0.043)</t>
   </si>
+  <si>
+    <t>83 total / 40 tha / 43 tka, 67.67 +-10.6 / 65.6+-10.6 tha / 69.6+-7.8 tka,male=44.57%/22.55%tha/15.35%tka, in TKA,32.3 +-5.7, in THA 27.8 +- 4.8</t>
+  </si>
+  <si>
+    <t>revised Temperament and Character Inventory</t>
+  </si>
+  <si>
+    <t>Pain
+Functionality
+Quality of life
+psychological factors</t>
+  </si>
+  <si>
+    <t>pain
+- Significant reductions in pain were reported at the 12-month follow-up (t5) in both THA and TKA patients (p &lt; 0.001).
+- There were no significant differences in pain (VAS scores) between THA and TKA patients at t5.
+- Residual pain (VAS &gt; 30 mm) at t5 was noted in 15% of THA patients and 25% of TKA patients, with no statistically significant difference between the two groups (p = 0.233).
+- Residual pain was correlated with SF-12 PCS (r2 = -0.412; p &lt; 0.001), SF-12 MCS (r2 = -0.473; p &lt; 0.001), HADS-A (r2 = 0.619; p &lt; 0.001), HADS-D (r2 = 0.559; p &lt; 0.001), functionality (r2 = -0.482; p &lt; 0.001) and WOMAC scores (r2 = 0.536; p &lt; 0.001) at t5.
+Functionality:
+- Significant functional improvement was reported at t5 in both THA and TKA patients (p &lt; 0.001).
+- THA patients showed earlier and greater functional improvement after surgery compared to TKA patients (p &lt; 0.001).
+- The largest amounts of variation were found in the functional scores (HHS=142.7% and KSS=182.5%)
+Quality of Life:
+- A significant time effect with a large effect size (ƞ2 &gt; 0.5) was noted for all variables except for the SF-12 MCS score (ƞ2 = 0.12).
+- Larger differences between pre- and post-operative scores at t5 were noted for the WOMAC score (THA = 80.5% vs TKA = 70.2%; p = 0.009) and SF-12 PCS score (THA = 57.4% vs TKA = 30.7%; p = 0.013)
+psychological factors
+- Higher pre-operative harm avoidance, persistence, and anxiety scores were predictive of residual pain after both THA and TKA (p &lt; 0.001). The logistic regression analysis showed that harm avoidance (p=0.034), persistence (p=0.003), and HADS-A scores (p=0.024) were significant predictors of residual pain.
+- There was a significant time effect noted for anxiety and depression scores, with improvement over time (p &lt; 0.001). The effect size was ƞ2 = 0.582 for anxiety, and ƞ2 = 0.377 for depression.</t>
+  </si>
+  <si>
+    <t>n=209 , age=72.84 (SD 8.32), male= 33%, BMI= 31.37 (SD 4.67)</t>
+  </si>
+  <si>
+    <t>WOMAC total 
+WOMAC pain
+WOMAC function
+KSS
+SF-12
+Anxiaty (STAI-X)</t>
+  </si>
+  <si>
+    <t>* The significance of the difference in the outcomes scores in the group with allergies was lost after adjusting for anxiety (p &gt; 0.05)
+* The State-Trait Anxiety Inventory (STAI-T) showed that anxiety was more prevalent in the group of patients with self-reported allergies (19.18 points) compared to the no allergy group (24.08 points), with a p-value of 0.039.
+* No significant differences were observed between the two groups for other psychiatric disorders assessed using the NEO-FFI (for neuroticism, extraversion, agreeableness, openness to experience, and conscientiousness), PHQ-15, PCS (total, rumination, magnification, helplessness), and RDQ
+- At 6 months follow up, the WOMAC total score improved less in the allergy group (34.37 points) compared to the no allergy group (40.10 points), with a p-value of 0.023.
+- The WOMAC pain score also improved less in the allergy group (6.03 points) compared to the no allergy group (7.50 points), with a p-value of 0.018
+- the WOMAC function score improved less in the allergy group (22.97 points) compared to the no allergy group (27.24 points), with a p-value of 0.023
+- The KSS-knee score improved less in the allergy group (25.37 points) than in the no allergy group (33.79 points), with a p-value of 0.002
+- The SF-12 physical score also showed less improvement in the allergy group (7.89 points) compared to the no allergy group (11.15 points), with a p-value of 0.046</t>
+  </si>
+  <si>
+    <t>n=80 ,mean age=66 , gender= 40%male ,NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient satisfaction
+VAS, WOMAC, Knee clinical score KSS, Function score KSS, ROM and Stability was used in order to measure satisfaction and dissatisfaction following operation
+</t>
+  </si>
+  <si>
+    <t>satisfation:    84% (72 patients) of patients reported being satisfied with their TKA, while 16% (14 patients) were dissatisfied.
+- Satisfied patients had a significantly lower mean VAS score (1.1 ± 1.5) compared to dissatisfied patients (6.7 ± 1.8) with a p-value of &lt;0.001
+-  Satisfied patients had a significantly lower mean WOMAC score (0.86 ± 1.3) compared to dissatisfied patients (5.76 ± 2.2) with a p-value of &lt;0.001
+- Satisfied patients had significantly better KSS scores (92 ± 13) compared to dissatisfied patients (65 ± 17), with a p-value of &lt;0.001
+- Satisfied patients had significantly better function scores (88 ± 16) co- mpared to dissatisfied patients (59 ± 22), with a p-value of &lt;0.001
+- There was no significant difference in ROM between satisfied (118° ± 11.4) and dissatisfied patients (117° ± 18.3), with a p-value of 0.262
+Personality Traits:
+- Life satisfaction: Satisfied patients showed significantly higher scores (9.5 ± 2.3) for life satisfaction compared to dissatisfied patients (7.4 ± 3.3) with a p-value of 0.006.
+- Performance orientation: Satisfied patients showed significantly higher scores (8.3 ± 2.5) for performance orientation compared to dissatisfied patients (6.5 ± 2.7) with a p-value of 0.015.
+- Somatic distress: Dissatisfied patients showed significantly higher scores (6.1 ± 3.2) for somatic distress compared to satisfied patients (3.4 ± 2.5) with a p-value of 0.001.
+- Emotional stability: Dissatisfied patients showed significantly higher scores (7.6 ± 4) for emotional instability compared to satisfied patients (4.4 ± 3.3) with a p-value of 0.002.
+- No significant differences were found in the other personality traits measured by the FPI-R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> to determine whether psychological factors affect health-related quality of life (HRQL) and recovery of knee function in total knee replacement (TKR) patients</t>
+  </si>
+  <si>
+    <t>STAI
+Beck Anxiety inventory
+Beck depression inventory
+The Knee Society Score (KSS), 
+The Short-Form Health Survey questionnaire (SF-36) are affected by negative emotions, including neuroticism, anxiety, and depression</t>
+  </si>
+  <si>
+    <t>n=387, age=59.6 +- 7.2 , male=28.37%, BMI=27.8 +- 4.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- Sanguine personalities had the best functional outcomes, and melancholic personalities had the worst functional outcomes.
+- The difference in SF-36 scores between the four personality types was significant (p &lt; 0.0001 for PCS and MCS).
+-There was a statistically significant negative association between extraversion and WOMAC scores and a significant positive association between neuroticism and WOMAC scores
+- The difference in WOMAC scores between the four personality types was significant (p = 0.0002 for pain, p = 0.0289 for stiffness, and p = 0.0058 for function)
+SF-36 PCS  and Extraversion 0.62 correlation p=0.040
+SF-36 MCS  and neuroticism -0.62 correlation p=0.018
+WOMAC pain Extraversion -0.64 correlation p=0.018
+WOMAC pain neuroticism -0.71 correlation p=0.025.
+Patient Satisfaction:
+- Overall patient satisfaction was assessed using a 100-mm visual analog scale (VAS).
+- Satisfaction rate showed a significant difference between the four personality types.
+- The percentage of sanguine patients was the highest, and the percentage of choleric patients was the lowest.
+</t>
+  </si>
+  <si>
+    <t>n=211. age=62.95,male=49.76% , bmi=26.99
+age:
+Choleric group: 62.3 (5.3)
+Sanguine group: 61.8 (6.1)
+Melancholic group: 60.4 (5.7)
+Phlegmatic group: 63.2 (5.5)
+BMI:
+Choleric group: 27.1 (3.1)
+Sanguine group: 26.8 (2.8)
+Melancholic group: 27.2 (3.2)
+Phlegmatic group: 27.0 (3.0)</t>
+  </si>
+  <si>
+    <t>costeffectiveness ratio (MCER), 
+quality-adjusted life years (QALYs), 
+McMaster Universities Osteoarthritis Index were measured (WOMAC) questionnaire, 
+EPQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Rheumatoid arthritis (RA) was significantly associated with a higher MCER (adjusted OR = 1.3, 95% CI = 1.2–1.4, P &lt; 0.01).
+American Society of Anesthesiologists (ASA) Class I-II was significantly associated with a lower MCER (adjusted OR = 0.9, 95% CI = 0.8–1.0, P &lt; 0.001).
+QALY
+There was a statistically significant difference in QALYs among the different personality traits (P &lt; 0.05).
+The sanguine group had the highest QALYs, with a mean of 6.9 (SD 1.3), while the melancholic group had the lowest QALYs, with a mean of 5.0 (SD 1.2).
+WOMAC
+There was a statistically significant difference in postoperative WOMAC scores among the different personality traits (P &lt; 0.05).
+The sanguine group had the lowest (best) postoperative WOMAC scores, with a mean of 37.9 (SD 9.2), whereas the melancholic group had the highest (worst) scores, with a mean of 51.7 (SD 8.2).
+There was a statistically significant difference in the change of total WOMAC scores among the different personality traits (P &lt; 0.05).
+The sanguine group showed the greatest improvement, with a mean change of 77.6 (SD 11.3), while the melancholic group showed the least improvement, with a mean change of 65.8 (SD 8.3).
+MCER
+There was a statistically significant difference in MCER among the different personality traits (P &lt; 0.05).
+The melancholic group had the highest MCER, with a mean of 3504.7 $/QALY (SD 576.2), indicating they would pay the highest costs for the same QALYs.
+The sanguine group had the lowest MCER, with a mean of 2264.0 $/QALY (SD 421.6), indicating they pay the least for the same QALYs.
+A sanguine personality was significantly associated with a lower MCER (adjusted OR = 0.8, 95% CI = 0.7–0.9, P &lt; 0.001).
+A melancholic personality was significantly associated with a higher MCER (adjusted OR = 1.2, 95% CI = 1.1–1.3, P &lt; 0.001).
+There were statistically significant differences in all of the cost categories among different personality groups (P &lt; 0.05), except for surgical procedures, where no significant difference was observed.
+The sanguine group had the lowest costs across all categories except for surgical procedures, and the melancholic group had the highest costs.</t>
+  </si>
+  <si>
+    <t>primary=488/revision=196,primary=67.4 +- 11.6 / revN=67.8+- 11.5,primary male=42.6% / revision male=46.9% , stratified percentages were reported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimism-Pessimism (PSM) scale of the Minnesota Multiphasic Personality Inventory
+(MMPI) questionnaire </t>
+  </si>
+  <si>
+    <t>moderate to severe pain
+Improvement in hip function
+Activity limitation</t>
+  </si>
+  <si>
+    <t>Primary THA Outcomes
+Moderate-Severe Pain:
+Pessimists showed a non-significant trend towards more moderate-severe pain at 2-years post-surgery compared to non-pessimists.
+- The odds ratio (OR) was 2.16 with a 95% confidence interval (CI) of (0.90, 5.20) and a p-value of 0.08.
+- 12.3% of pessimists reported moderate-severe pain compared to 8.6% of non-pessimists.
+Improvement in Hip Function:
+There was no significant difference in the absence of "much better" improvement in hip function at 2-years between pessimists and non-pessimists.
+- The odds ratio (OR) was 1.87 with a 95% confidence interval (CI) of (0.77, 4.52) and a p-value of 0.16.
+- 17.6% of pessimists reported a lack of "much better" improvement compared to 12.7% of non-pessimists.
+Moderate-Severe Activity Limitation:
+- Pessimists reported a significantly higher rate of moderate-severe activity limitation at 2-years post-surgery.
+- The odds ratio (OR) was 2.90 with a 95% confidence interval (CI) of (1.25, 6.70) and a p-value of 0.01. This result was statistically significant even when using an adjusted p-value threshold of 0.017 for multiple comparisons.
+- 42.2% of pessimists reported moderate-severe activity limitation compared to 32.4% of non-pessimists.
+Revision THA Outcomes
+Moderate-Severe Pain:
+There was no significant difference between pessimists and non-pessimists in reporting moderate-severe pain at 2 years post-revision THA.
+- The odds ratio (OR) was 1.18 with a 95% confidence interval (CI) of (0.50, 2.81) and a p-value of 0.71.
+Improvement in Hip Function:
+There was no significant difference between pessimists and non-pessimists in reporting "much better" improvement in hip function at 2 years post-revision THA.
+- The odds ratio (OR) was 1.08 with a 95% confidence interval (CI) of (0.52, 2.27) and a p-value of 0.83.
+Moderate-Severe Activity Limitation:
+There was no significant difference between pessimists and non-pessimists in reporting moderate-severe activity limitation at 2 years post-revision THA.
+- The odds ratio (OR) was 1.73 with a 95% confidence interval (CI) of (0.76, 3.94) and a p-value of 0.19</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -977,35 +1032,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B0F0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="4"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1160,16 +1186,13 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1194,31 +1217,19 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1226,24 +1237,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1253,6 +1246,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1477,8 +1479,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1495,877 +1497,877 @@
     <col min="11" max="11" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:26" s="3" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="7" customFormat="1" ht="220.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:26" s="4" customFormat="1" ht="220.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="13">
+        <v>9</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="13">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:26" s="4" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J4" s="13">
+        <v>9</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="13">
+        <v>29</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:26" s="4" customFormat="1" ht="331.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" s="13">
+        <v>10</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="13">
+        <v>28</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="1:26" s="3" customFormat="1" ht="331.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J6" s="16">
+        <v>11</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="14">
+        <v>9</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="3" customFormat="1" ht="234.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" s="16">
+        <v>8</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="193.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="J9" s="13">
+        <v>13</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="13">
+        <v>22</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+    </row>
+    <row r="10" spans="1:26" s="3" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J10" s="18">
+        <v>10</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="18">
+        <v>19</v>
+      </c>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+    </row>
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="317.39999999999998" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" s="13">
+        <v>7</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" s="13">
+        <v>18</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+    </row>
+    <row r="12" spans="1:26" s="3" customFormat="1" ht="345" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="J12" s="16">
+        <v>10</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="3" customFormat="1" ht="220.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="J13" s="16">
+        <v>9</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="3" customFormat="1" ht="234.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="J14" s="16">
+        <v>10</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="14">
+        <v>8</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="4" customFormat="1" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J16" s="13">
+        <v>11</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="13">
+        <v>10</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+    </row>
+    <row r="17" spans="1:26" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="1:26" s="4" customFormat="1" ht="262.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="J18" s="13">
+        <v>10</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="L18" s="13">
+        <v>13</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+    </row>
+    <row r="19" spans="1:26" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+    </row>
+    <row r="20" spans="1:26" s="4" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="J2" s="16">
+      <c r="D20" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="J20" s="13">
         <v>9</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K20" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="L20" s="13">
         <v>16</v>
       </c>
-      <c r="L2" s="16">
-        <v>32</v>
-      </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-    </row>
-    <row r="4" spans="1:26" s="7" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="J4" s="16">
+    <row r="21" spans="1:26" s="3" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="J21" s="20">
         <v>9</v>
       </c>
-      <c r="K4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="16">
-        <v>29</v>
-      </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-    </row>
-    <row r="5" spans="1:26" s="7" customFormat="1" ht="331.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="J5" s="16">
-        <v>10</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="16">
-        <v>28</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-    </row>
-    <row r="6" spans="1:26" s="6" customFormat="1" ht="331.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="J6" s="23">
-        <v>11</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="23">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="17">
-        <v>9</v>
-      </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="6" customFormat="1" ht="234.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="J8" s="23">
-        <v>8</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" s="23">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="7" customFormat="1" ht="207" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="J9" s="16">
-        <v>13</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" s="16">
-        <v>22</v>
-      </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-    </row>
-    <row r="10" spans="1:26" s="6" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="J10" s="31">
-        <v>10</v>
-      </c>
-      <c r="K10" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="L10" s="31">
-        <v>19</v>
-      </c>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="32"/>
-    </row>
-    <row r="11" spans="1:26" s="7" customFormat="1" ht="317.39999999999998" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="J11" s="16">
-        <v>7</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="L11" s="16">
-        <v>18</v>
-      </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-    </row>
-    <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="21">
-        <v>10</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="L12" s="21">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="J13" s="21">
-        <v>9</v>
-      </c>
-      <c r="K13" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="L13" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="21">
-        <v>10</v>
-      </c>
-      <c r="K14" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="L14" s="21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15" s="17">
-        <v>8</v>
-      </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" s="19">
-        <v>11</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="L16" s="19">
-        <v>10</v>
-      </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-    </row>
-    <row r="17" spans="1:26" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-    </row>
-    <row r="18" spans="1:26" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="J18" s="19">
-        <v>10</v>
-      </c>
-      <c r="K18" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="L18" s="19">
-        <v>13</v>
-      </c>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-    </row>
-    <row r="19" spans="1:26" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-    </row>
-    <row r="20" spans="1:26" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="H20" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="I20" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="J20" s="19">
-        <v>9</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="L20" s="19">
-        <v>16</v>
-      </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-    </row>
-    <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="J21" s="28">
-        <v>9</v>
-      </c>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28">
+      <c r="K21" s="20"/>
+      <c r="L21" s="20">
         <v>2</v>
       </c>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>